<commit_message>
LSH 和 Minhash review
</commit_message>
<xml_diff>
--- a/博客-文章/石晓文/目录.xlsx
+++ b/博客-文章/石晓文/目录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmy/workspace/reference/note/博客-文章/石晓文/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A23C4DE-26DC-B647-B759-7C5D0FBE83DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2263AB1-027C-9046-B15B-503A022F1E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10340" yWindow="4280" windowWidth="20000" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="200">
   <si>
     <t>title</t>
   </si>
@@ -659,6 +659,10 @@
   </si>
   <si>
     <t>没看需要对抗网络</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deep Neural Networks for YouTube Recommendations</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1629,10 +1633,10 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2493,6 +2497,9 @@
       <c r="H35" t="s">
         <v>183</v>
       </c>
+      <c r="I35" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">

</xml_diff>

<commit_message>
youtube 2016 DNN 完成
</commit_message>
<xml_diff>
--- a/博客-文章/石晓文/目录.xlsx
+++ b/博客-文章/石晓文/目录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmy/workspace/reference/note/博客-文章/石晓文/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5E1F7E-0EA2-BA43-9090-20ABC5473830}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB2461D-FA3C-E243-8719-CDC839D1F0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11400" yWindow="4280" windowWidth="18940" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="201">
   <si>
     <t>title</t>
   </si>
@@ -218,9 +218,6 @@
     <t>2019.03.14</t>
   </si>
   <si>
-    <t>推荐系统遇上深度学习(三十六)--Learning and Transferring IDs Representation in E-commerce</t>
-  </si>
-  <si>
     <t>2019.04.04</t>
   </si>
   <si>
@@ -242,13 +239,7 @@
     <t>2019.05.09</t>
   </si>
   <si>
-    <t>推荐系统遇上深度学习(四十三)-考虑用户微观行为的电商推荐</t>
-  </si>
-  <si>
     <t>2019.05.10</t>
-  </si>
-  <si>
-    <t>推荐系统遇上深度学习(四十四)-Airbnb实时搜索排序中的Embedding技巧</t>
   </si>
   <si>
     <t>2019.05.12</t>
@@ -634,10 +625,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>没看代码</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>推荐系统遇上深度学习(三十八)--CFGAN:一种基于GAN的协同过滤推荐框架</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -674,11 +661,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>没实现</t>
+    <t>没看，基于序列的推荐</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>没看，基于序列的推荐</t>
+    <t>推荐系统遇上深度学习(四十三)-考虑用户微观行为的电商推荐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>推荐系统遇上深度学习(四十四)-Airbnb实时搜索排序中的Embedding技巧</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>推荐系统遇上深度学习(三十六)--Learning and Transferring IDs Representation in E-commerce</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1665,10 +1660,10 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1682,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1889,7 +1884,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -1936,10 +1931,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
@@ -1962,7 +1957,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1986,10 +1981,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>27</v>
@@ -2015,7 +2010,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>29</v>
@@ -2041,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
@@ -2062,7 +2057,7 @@
         <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2070,7 +2065,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
@@ -2093,10 +2088,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
@@ -2167,10 +2162,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -2193,7 +2188,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
@@ -2216,10 +2211,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -2245,7 +2240,7 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C24" t="s">
         <v>43</v>
@@ -2268,10 +2263,10 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
@@ -2294,10 +2289,10 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -2311,7 +2306,7 @@
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
@@ -2334,7 +2329,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>
@@ -2360,7 +2355,7 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
@@ -2383,10 +2378,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
@@ -2412,7 +2407,7 @@
         <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>53</v>
@@ -2435,10 +2430,10 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>54</v>
@@ -2464,7 +2459,7 @@
         <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>56</v>
@@ -2487,10 +2482,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>57</v>
@@ -2513,11 +2508,9 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>201</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="B35" s="6"/>
       <c r="C35" s="2" t="s">
         <v>58</v>
       </c>
@@ -2537,14 +2530,16 @@
         <v>53</v>
       </c>
       <c r="I35" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="C36" s="2" t="s">
         <v>60</v>
       </c>
@@ -2564,18 +2559,16 @@
         <v>22</v>
       </c>
       <c r="I36" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D37" s="4">
         <v>0.9868055555555556</v>
@@ -2595,13 +2588,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="4">
         <v>0.96666666666666667</v>
@@ -2621,13 +2614,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D39" s="4">
         <v>0.88263888888888886</v>
@@ -2647,13 +2640,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D40" s="4">
         <v>0.69166666666666676</v>
@@ -2673,13 +2666,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B41" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="1">
         <v>0.73472222222222217</v>
@@ -2699,13 +2692,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B42" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="1">
         <v>0.80833333333333324</v>
@@ -2725,10 +2718,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>195</v>
+      </c>
+      <c r="B43" t="s">
+        <v>194</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="1">
         <v>0.92222222222222217</v>
@@ -2748,10 +2744,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>198</v>
+      </c>
+      <c r="B44" t="s">
+        <v>194</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D44" s="1">
         <v>0.73611111111111116</v>
@@ -2771,10 +2770,10 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>199</v>
       </c>
       <c r="C45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D45" s="1">
         <v>0.91736111111111107</v>
@@ -2794,10 +2793,10 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D46" s="1">
         <v>0.53402777777777777</v>
@@ -2817,10 +2816,10 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D47" s="1">
         <v>0.59861111111111109</v>
@@ -2840,10 +2839,10 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D48" s="1">
         <v>6.9444444444444447E-4</v>
@@ -2863,10 +2862,10 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D49" s="1">
         <v>9.0277777777777787E-3</v>
@@ -2886,10 +2885,10 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D50" s="1">
         <v>0.68125000000000002</v>
@@ -2909,11 +2908,11 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D51" s="4">
         <v>0.75138888888888899</v>
@@ -2933,11 +2932,11 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D52" s="4">
         <v>0.44791666666666669</v>
@@ -2957,11 +2956,11 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D53" s="4">
         <v>0.91041666666666676</v>
@@ -2981,11 +2980,11 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D54" s="4">
         <v>0.72638888888888886</v>
@@ -3005,11 +3004,11 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D55" s="4">
         <v>0.97569444444444453</v>
@@ -3029,11 +3028,11 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D56" s="4">
         <v>0.97152777777777777</v>
@@ -3053,11 +3052,11 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D57" s="4">
         <v>0.90277777777777779</v>
@@ -3077,11 +3076,11 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D58" s="4">
         <v>0.94513888888888886</v>
@@ -3101,11 +3100,11 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D59" s="4">
         <v>0.7090277777777777</v>
@@ -3125,11 +3124,11 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D60" s="4">
         <v>0.93055555555555547</v>
@@ -3149,10 +3148,10 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D61" s="1">
         <v>0.69305555555555554</v>
@@ -3172,10 +3171,10 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D62" s="1">
         <v>0.43472222222222223</v>
@@ -3195,10 +3194,10 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D63" s="1">
         <v>0.63194444444444442</v>
@@ -3218,10 +3217,10 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D64" s="1">
         <v>0.55972222222222223</v>
@@ -3241,10 +3240,10 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D65" s="1">
         <v>0.71666666666666667</v>
@@ -3264,10 +3263,10 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D66" s="1">
         <v>0.73333333333333339</v>
@@ -3287,10 +3286,10 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D67" s="1">
         <v>0.53611111111111109</v>
@@ -3310,10 +3309,10 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D68" s="1">
         <v>0.99513888888888891</v>
@@ -3333,10 +3332,10 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D69" s="1">
         <v>0.79861111111111116</v>
@@ -3356,10 +3355,10 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D70" s="1">
         <v>0.97986111111111107</v>
@@ -3379,11 +3378,11 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D71" s="4">
         <v>0.4284722222222222</v>
@@ -3403,11 +3402,11 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D72" s="4">
         <v>0.50138888888888888</v>
@@ -3427,11 +3426,11 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D73" s="4">
         <v>0.9159722222222223</v>
@@ -3451,11 +3450,11 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D74" s="4">
         <v>0.70277777777777783</v>
@@ -3475,11 +3474,11 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D75" s="4">
         <v>0.76250000000000007</v>
@@ -3499,11 +3498,11 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D76" s="4">
         <v>0.69930555555555562</v>
@@ -3523,11 +3522,11 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D77" s="4">
         <v>0.77916666666666667</v>
@@ -3547,11 +3546,11 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D78" s="4">
         <v>0.85138888888888886</v>
@@ -3571,11 +3570,11 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D79" s="4">
         <v>0.67847222222222225</v>
@@ -3595,11 +3594,11 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D80" s="4">
         <v>0.95416666666666661</v>
@@ -3619,10 +3618,10 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D81" s="1">
         <v>0.88888888888888884</v>
@@ -3642,10 +3641,10 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C82" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D82" s="1">
         <v>0.78680555555555554</v>
@@ -3665,10 +3664,10 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D83" s="1">
         <v>0.6118055555555556</v>
@@ -3688,10 +3687,10 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C84" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D84" s="1">
         <v>0.62222222222222223</v>
@@ -3711,10 +3710,10 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D85" s="1">
         <v>0.84097222222222223</v>
@@ -3734,10 +3733,10 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C86" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D86" s="1">
         <v>0.8833333333333333</v>
@@ -3757,10 +3756,10 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C87" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D87" s="1">
         <v>0.70347222222222217</v>
@@ -3780,10 +3779,10 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C88" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D88" s="1">
         <v>0.90069444444444446</v>
@@ -3803,7 +3802,7 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C89">
         <v>8.01</v>
@@ -3826,7 +3825,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C90">
         <v>8.02</v>
@@ -3849,7 +3848,7 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2">
@@ -3873,7 +3872,7 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2">
@@ -3897,7 +3896,7 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2">
@@ -3921,7 +3920,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2">
@@ -3945,7 +3944,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2">
@@ -3969,7 +3968,7 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2">
@@ -3993,7 +3992,7 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2">

</xml_diff>